<commit_message>
fixed Game Over bug
</commit_message>
<xml_diff>
--- a/game_template/model/data/floor builder Level 4.xlsx
+++ b/game_template/model/data/floor builder Level 4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7770" windowHeight="540" tabRatio="904" firstSheet="4" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7770" windowHeight="540" tabRatio="904" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Reverser" sheetId="33" r:id="rId1"/>
@@ -1965,35 +1965,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="67">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="65">
     <dxf>
       <fill>
         <patternFill>
@@ -2026,6 +1998,20 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5148,12 +5134,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="66" priority="2">
+    <cfRule type="expression" dxfId="64" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="65" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6941,22 +6927,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y20 A22:Y25 U21:Y21">
-    <cfRule type="expression" dxfId="30" priority="4">
+    <cfRule type="expression" dxfId="26" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z20 A22:Z25 U21:Z21">
-    <cfRule type="cellIs" dxfId="29" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="expression" dxfId="28" priority="2">
+    <cfRule type="expression" dxfId="24" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8744,22 +8730,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22:Y25 U21:Y21 A1:Y20">
-    <cfRule type="expression" dxfId="26" priority="4">
+    <cfRule type="expression" dxfId="22" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:Z25 U21:Z21 A1:Z20">
-    <cfRule type="cellIs" dxfId="25" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="cellIs" dxfId="23" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8772,7 +8758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB20" sqref="AB1:AB20"/>
     </sheetView>
   </sheetViews>
@@ -10547,22 +10533,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22:Y25 U21:Y21 A1:Y20">
-    <cfRule type="expression" dxfId="22" priority="4">
+    <cfRule type="expression" dxfId="18" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:Z25 U21:Z21 A1:Z20">
-    <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="expression" dxfId="20" priority="2">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="cellIs" dxfId="19" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12350,22 +12336,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22:Y25 U21:Y21 A1:Y1 A5:Y20 A2:H4 L2:Y4">
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="14" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:Z25 U21:Z21 A1:Z1 A5:Z20 A2:H4 L2:Z4">
-    <cfRule type="cellIs" dxfId="17" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="expression" dxfId="16" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="cellIs" dxfId="15" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14153,22 +14139,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22:Y25 U21:Y21 A1:Y20">
-    <cfRule type="expression" dxfId="14" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:Z25 U21:Z21 A1:Z20">
-    <cfRule type="cellIs" dxfId="13" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16036,22 +16022,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Y20 A21:Z25">
-    <cfRule type="cellIs" dxfId="9" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:Z20">
-    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:Z20">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18223,17 +18209,17 @@
     <sortCondition ref="B2:B66"/>
   </sortState>
   <conditionalFormatting sqref="D1:D65 D67:D1048576">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K65">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D66">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20020,22 +20006,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y20 A22:Y25 U21:Y21">
-    <cfRule type="expression" dxfId="64" priority="4">
+    <cfRule type="expression" dxfId="62" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z20 A22:Z25 U21:Z21">
-    <cfRule type="cellIs" dxfId="63" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="expression" dxfId="62" priority="2">
+    <cfRule type="expression" dxfId="60" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="cellIs" dxfId="61" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21823,22 +21809,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y20 A22:Y25 U21:Y21">
-    <cfRule type="expression" dxfId="60" priority="4">
+    <cfRule type="expression" dxfId="58" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z20 A22:Z25 U21:Z21">
-    <cfRule type="cellIs" dxfId="59" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="expression" dxfId="58" priority="2">
+    <cfRule type="expression" dxfId="56" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="cellIs" dxfId="57" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23706,42 +23692,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:T20 A22:Y25 U21:Y21 V1:Y20">
-    <cfRule type="expression" dxfId="56" priority="8">
+    <cfRule type="expression" dxfId="54" priority="8">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20 A22:Z25 U21:Z21 V1:Y20">
-    <cfRule type="cellIs" dxfId="55" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="7" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="expression" dxfId="54" priority="6">
+    <cfRule type="expression" dxfId="52" priority="6">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="cellIs" dxfId="53" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="5" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U20">
-    <cfRule type="expression" dxfId="52" priority="4">
+    <cfRule type="expression" dxfId="50" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U20">
-    <cfRule type="cellIs" dxfId="51" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:Z20">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="48" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:Z20">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25529,22 +25515,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22:Y25 U21:Y21 A1:Y20">
-    <cfRule type="expression" dxfId="50" priority="4">
+    <cfRule type="expression" dxfId="46" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:Z25 U21:Z21 A1:Z20">
-    <cfRule type="cellIs" dxfId="49" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="expression" dxfId="48" priority="2">
+    <cfRule type="expression" dxfId="44" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="cellIs" dxfId="47" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27332,22 +27318,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22:Y25 U21:Y21 A1:Y20">
-    <cfRule type="expression" dxfId="46" priority="4">
+    <cfRule type="expression" dxfId="42" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:Z25 U21:Z21 A1:Z20">
-    <cfRule type="cellIs" dxfId="45" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="expression" dxfId="44" priority="2">
+    <cfRule type="expression" dxfId="40" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="cellIs" dxfId="43" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29134,22 +29120,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22:Y25 U21:Y21 A1:Y20">
-    <cfRule type="expression" dxfId="42" priority="4">
+    <cfRule type="expression" dxfId="38" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:Z25 U21:Z21 A1:Z20">
-    <cfRule type="cellIs" dxfId="41" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="expression" dxfId="40" priority="2">
+    <cfRule type="expression" dxfId="36" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="cellIs" dxfId="39" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29162,8 +29148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AB20" sqref="AB1:AB20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29607,7 +29593,7 @@
         <v>6</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
@@ -29616,11 +29602,11 @@
       <c r="Y6" s="7"/>
       <c r="AA6" t="str">
         <f t="shared" si="0"/>
-        <v>w:                 :</v>
+        <v>w:                 /</v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="1"/>
-        <v>'w:                 :',</v>
+        <v>'w:                 /',</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -30936,22 +30922,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22:Y25 U21:Y21 A1:Y20">
-    <cfRule type="expression" dxfId="38" priority="4">
+    <cfRule type="expression" dxfId="34" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:Z25 U21:Z21 A1:Z20">
-    <cfRule type="cellIs" dxfId="37" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="expression" dxfId="36" priority="2">
+    <cfRule type="expression" dxfId="32" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="cellIs" dxfId="35" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32739,22 +32725,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y20 A22:Y25 U21:Y21">
-    <cfRule type="expression" dxfId="34" priority="4">
+    <cfRule type="expression" dxfId="30" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z20 A22:Z25 U21:Z21">
-    <cfRule type="cellIs" dxfId="33" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="expression" dxfId="32" priority="2">
+    <cfRule type="expression" dxfId="28" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="cellIs" dxfId="31" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>